<commit_message>
Added different data to xlsx file to confirm we are reading the correct file
</commit_message>
<xml_diff>
--- a/savvy.xlsx
+++ b/savvy.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garyanewsome/Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garyanewsome/Projects/Health-Payer-Processor/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Gary</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Just proving we are reading the correct documents</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,6 +473,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>